<commit_message>
This is full development fot automation framework
</commit_message>
<xml_diff>
--- a/Externaldata/CamsEntry.xlsx
+++ b/Externaldata/CamsEntry.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nirak\Desktop\Radhakrushna_OASYS\Cams_Oasys\Externaldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E99CD1C-2D2D-457D-BFBE-B5219DE8A92F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76697113-2F5C-4803-9CE4-EBD13B9C6B3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{1C652985-6E6C-4A4D-8ADE-F8717E9CC80D}"/>
   </bookViews>
@@ -34,90 +34,96 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="28">
-  <si>
-    <t>Firstname</t>
-  </si>
-  <si>
-    <t>Lastname</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
   <si>
     <t>EmailId</t>
   </si>
   <si>
-    <t>Phone No</t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>State</t>
-  </si>
-  <si>
     <t>District</t>
   </si>
   <si>
-    <t>City</t>
-  </si>
-  <si>
     <t>Address</t>
   </si>
   <si>
-    <t>Pincode</t>
-  </si>
-  <si>
-    <t>Olanda</t>
-  </si>
-  <si>
-    <t>Sargaon</t>
-  </si>
-  <si>
-    <t>Oasys</t>
-  </si>
-  <si>
     <t>Cams@1234</t>
   </si>
   <si>
-    <t>OlandaSargaon</t>
-  </si>
-  <si>
-    <t>INDIA</t>
-  </si>
-  <si>
-    <t>ODISHA</t>
-  </si>
-  <si>
-    <t>BALASORE</t>
-  </si>
-  <si>
-    <t>Ganjam</t>
-  </si>
-  <si>
-    <t>Aska</t>
-  </si>
-  <si>
-    <t>A.Karadabadi</t>
-  </si>
-  <si>
-    <t>Cams@1235</t>
-  </si>
-  <si>
-    <t>Sambalpur</t>
-  </si>
-  <si>
-    <t>A.Katapali</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A.Karadabadi </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> A.Katapali </t>
-  </si>
-  <si>
-    <t>SCS</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Division</t>
+  </si>
+  <si>
+    <t>Circle</t>
+  </si>
+  <si>
+    <t>Block_ULB</t>
+  </si>
+  <si>
+    <t>BranchName</t>
+  </si>
+  <si>
+    <t>CCB</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Aida SCS</t>
+  </si>
+  <si>
+    <t>admin209@gmail.com</t>
+  </si>
+  <si>
+    <t>At/Po-Aida</t>
+  </si>
+  <si>
+    <t>Angul</t>
+  </si>
+  <si>
+    <t>Athamallik</t>
+  </si>
+  <si>
+    <t>ANGUL UCCB</t>
+  </si>
+  <si>
+    <t>PACS</t>
+  </si>
+  <si>
+    <t>Ambasarmunda SCS</t>
+  </si>
+  <si>
+    <t>At/Po-Ambasarmunda</t>
+  </si>
+  <si>
+    <t>Angapada SCS</t>
+  </si>
+  <si>
+    <t>admin258@gmail.com</t>
+  </si>
+  <si>
+    <t>At/Po-Angapada</t>
+  </si>
+  <si>
+    <t>Kishorenagar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Boinda </t>
+  </si>
+  <si>
+    <t>Login_Status</t>
+  </si>
+  <si>
+    <t>successfully login</t>
+  </si>
+  <si>
+    <t>admin24@gmail.com</t>
+  </si>
+  <si>
+    <t>not login successfully...</t>
   </si>
 </sst>
 </file>
@@ -125,7 +131,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="0"/>
-  <fonts count="7">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -140,18 +146,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -181,12 +175,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -194,50 +188,23 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="5">
-    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
+  <cellStyles count="4">
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="2" xr:uid="{2EBA781F-317D-4C62-876B-8EDCC9F52333}"/>
-    <cellStyle name="Normal 4" xfId="3" xr:uid="{2DAD7EF9-5B50-40E9-83D2-17E51B32096E}"/>
-    <cellStyle name="Normal_Sheet1" xfId="1" xr:uid="{53A72F2E-E28D-402E-9D88-26D21CB07477}"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{2EBA781F-317D-4C62-876B-8EDCC9F52333}"/>
+    <cellStyle name="Normal 4" xfId="2" xr:uid="{2DAD7EF9-5B50-40E9-83D2-17E51B32096E}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -549,10 +516,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1850ACB-5F58-4CAF-9DC7-5F6B0A795763}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:L4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -568,151 +535,164 @@
     <col min="9" max="9" customWidth="true" width="15.21875"/>
     <col min="10" max="10" customWidth="true" width="16.0"/>
     <col min="11" max="11" customWidth="true" width="17.77734375"/>
+    <col min="12" max="12" customWidth="true" width="29.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12" s="1" customFormat="1">
       <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" t="s">
+        <v>17</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" t="s">
+        <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:11">
-      <c r="A2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="3">
-        <v>1234567890</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" s="3" t="s">
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H3" t="s">
+        <v>16</v>
+      </c>
+      <c r="I3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J3" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="K3" t="s">
         <v>18</v>
       </c>
-      <c r="I2" s="2" t="s">
+      <c r="L3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K4" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="K2" s="3">
-        <v>756027</v>
-      </c>
-    </row>
-    <row r="3" spans="1:11">
-      <c r="A3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B3" s="3" t="s">
+      <c r="L4" t="s">
         <v>27</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="3">
-        <v>1234567890</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="K3" s="3">
-        <v>761118</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11">
-      <c r="A4" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3">
-        <v>1234567890</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K4" s="3">
-        <v>768006</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{3A964E58-3D35-43DE-847A-9DCF76A25E1B}"/>
+    <hyperlink ref="B3" r:id="rId1" xr:uid="{6146078E-71CB-4BC2-A777-5D812A73054E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>